<commit_message>
Updates to scaling mappings and scaling rules
</commit_message>
<xml_diff>
--- a/input/mappings/fuel_sector_ash_retention_mapping.xlsx
+++ b/input/mappings/fuel_sector_ash_retention_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="100" windowWidth="16060" windowHeight="13060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="300" yWindow="100" windowWidth="16060" windowHeight="13060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="fuel" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>2D_Paint-application</t>
   </si>
   <si>
-    <t>2D3_Chemical-product-use</t>
-  </si>
-  <si>
     <t>2H_Pulp-and-paper-food-beverage-wood</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>1A4b_Residential</t>
+  </si>
+  <si>
+    <t>2D3_Chemical-products-manufacture-processing</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D25" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1116,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1135,7 +1135,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1143,7 +1143,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1255,7 +1255,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1271,7 +1271,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1279,7 +1279,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1287,7 +1287,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1295,7 +1295,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1303,7 +1303,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1311,7 +1311,7 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1319,7 +1319,7 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1327,7 +1327,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1335,7 +1335,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1343,7 +1343,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>